<commit_message>
Updated the template file.
</commit_message>
<xml_diff>
--- a/hcm/houseCodeRequest/usr/HouseCodeRequest.xlsx
+++ b/hcm/houseCodeRequest/usr/HouseCodeRequest.xlsx
@@ -1109,12 +1109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1392,11 +1391,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,28 +1456,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1488,9 +1465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DM1"/>
   <sheetViews>
-    <sheetView topLeftCell="DS1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="DZ42" sqref="DZ42"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,11 +1477,10 @@
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="17" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="37.140625" customWidth="1"/>
@@ -1924,9 +1900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GH1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="CD2" sqref="A2:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,7 +2717,7 @@
   <dimension ref="A1:C709"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2888,11 +2864,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>42327</v>
+        <v>42361</v>
       </c>
       <c r="B2">
         <f ca="1">(YEAR(DATE!A2)-2000+100)*1000+DATE!A2-DATE(YEAR(DATE!A2),"01","01")+1</f>
-        <v>115323</v>
+        <v>115357</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>

</xml_diff>